<commit_message>
[Silverfox] 19_TrashYard ~19_023까지 저장 / 사운드 발주문서 / Tube_Style
</commit_message>
<xml_diff>
--- a/DesignDocs/Design/발주 문서/사운드 발주 문서.xlsx
+++ b/DesignDocs/Design/발주 문서/사운드 발주 문서.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\Design\발주 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E691E98-ED2D-4F3E-9008-6C51F2C6FC2A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1004D3A-4F5B-49A1-8A3F-8229F649CDCF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11190" xr2:uid="{18E5C2E1-74D7-4506-AC11-C835359D26D8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11190" firstSheet="1" activeTab="2" xr2:uid="{18E5C2E1-74D7-4506-AC11-C835359D26D8}"/>
   </bookViews>
   <sheets>
     <sheet name="PC" sheetId="2" r:id="rId1"/>
     <sheet name="Rat" sheetId="3" r:id="rId2"/>
     <sheet name="Hyena" sheetId="5" r:id="rId3"/>
     <sheet name="Mearcat" sheetId="6" r:id="rId4"/>
-    <sheet name="Machine" sheetId="4" r:id="rId5"/>
+    <sheet name="DonCina" sheetId="7" r:id="rId5"/>
+    <sheet name="Machine" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="128">
   <si>
     <t>순번</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -205,10 +206,6 @@
   </si>
   <si>
     <t>점프 시작시 발 디딛고, 뱅글 도는 사운드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>걷는 소리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -366,6 +363,161 @@
   </si>
   <si>
     <t>와장창 + 굴파는 소리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>걷기 - 중형 / 단단한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rat_02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금속 나사를 슬링으로 던져서 맞는 소리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DonCina</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idle_01</t>
+  </si>
+  <si>
+    <t>Idle_BT</t>
+  </si>
+  <si>
+    <t>Walk_01</t>
+  </si>
+  <si>
+    <t>Jump_01</t>
+  </si>
+  <si>
+    <t>Dameged_01</t>
+  </si>
+  <si>
+    <t>Die</t>
+  </si>
+  <si>
+    <t>Skill_00</t>
+  </si>
+  <si>
+    <t>Skill_01</t>
+  </si>
+  <si>
+    <t>대기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발구르기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발 구르기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>걷기 - 대형 / 단단한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>점프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피격</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사망 - 대형</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사슬 휘두르기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사슬 내던지기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사슬을 위에서 아래로 내리는 소리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사슬을 적에게 내던지는 소리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타격 - 사슬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill_00 / Skill_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>찰그락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사슬 회수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skill_01에 맞으면 사슬을 당기는 촤르륵 소리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hyena_02</t>
+  </si>
+  <si>
+    <t>대기 - 물뿌리기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작은 물 뿌리는 소리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대기 - 펌프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>펌프 소리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사망 - 중형</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물줄기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물줄기 내보내는 소리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타격 - 물줄기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물줄기 맞는 소리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -738,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5DCCB71-CB7F-462B-A010-27FB097CD8A0}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -874,7 +1026,7 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -978,10 +1130,10 @@
         <v>46</v>
       </c>
       <c r="D15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" t="s">
         <v>48</v>
-      </c>
-      <c r="E15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -992,13 +1144,13 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1010,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5309C050-7EEF-4E87-8044-39DA8BE020A9}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1046,13 +1198,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1060,16 +1212,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
         <v>55</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>56</v>
-      </c>
-      <c r="E3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1077,16 +1229,16 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
         <v>58</v>
-      </c>
-      <c r="E4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1094,16 +1246,16 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
         <v>61</v>
-      </c>
-      <c r="E5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1111,16 +1263,16 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1128,16 +1280,16 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1145,16 +1297,33 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>68</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>69</v>
       </c>
-      <c r="E8" t="s">
-        <v>70</v>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1165,7 +1334,210 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA137FF9-B0D7-4DA0-A2AD-76F2B11C5B5B}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.25" customWidth="1"/>
+    <col min="3" max="3" width="23.875" customWidth="1"/>
+    <col min="4" max="4" width="21.75" customWidth="1"/>
+    <col min="5" max="5" width="40.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95C82AD-A408-404C-BBEF-C5CB7C06D69B}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
@@ -1196,35 +1568,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" t="s">
-        <v>75</v>
+        <v>82</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1232,50 +1607,16 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1284,12 +1625,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B95C82AD-A408-404C-BBEF-C5CB7C06D69B}">
-  <dimension ref="A1:E4"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5DAA55-595A-4596-A207-07AF1825F82F}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1317,47 +1658,166 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>87</v>
-      </c>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1365,7 +1825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3321063-C5CB-428A-8A88-37DE821C7A64}">
   <dimension ref="A1:E1"/>
   <sheetViews>

</xml_diff>